<commit_message>
Todd update syllabus and TAM
</commit_message>
<xml_diff>
--- a/ABM_Syllabus.xlsx
+++ b/ABM_Syllabus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Desktop\ABM class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Desktop\OSU_Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B23829F-24AF-461E-910B-F6A2263F6B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00469F7A-9500-422A-9F18-1C870D176161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21075" yWindow="1110" windowWidth="23475" windowHeight="13680" xr2:uid="{E5130AA3-D4D3-4EA2-831A-5461D6EB2535}"/>
+    <workbookView xWindow="1170" yWindow="135" windowWidth="28950" windowHeight="15465" xr2:uid="{E5130AA3-D4D3-4EA2-831A-5461D6EB2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Day</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>Documenting models</t>
-  </si>
-  <si>
     <t>Ch. 3, Supplemental</t>
   </si>
   <si>
@@ -85,15 +82,9 @@
     <t>Course Feedback, moving forward with models</t>
   </si>
   <si>
-    <t>Lecture: What are models? Why do we use them? Intro to Netlogo</t>
-  </si>
-  <si>
     <t>Exercise: Getting familiar with Netlogo</t>
   </si>
   <si>
-    <t>Conceptual Modeling</t>
-  </si>
-  <si>
     <t>Exercise: Conceptual Modeling</t>
   </si>
   <si>
@@ -112,45 +103,27 @@
     <t>Chpt. 3</t>
   </si>
   <si>
-    <t>Model Evaluation &amp; Pattern oriented modeling</t>
-  </si>
-  <si>
     <t>Break for evening (Homework: Netlogo dictionary, ODD: design questions)</t>
   </si>
   <si>
-    <t>Conceptual model presentations</t>
-  </si>
-  <si>
     <t>Chpts. 6, 4, 5</t>
   </si>
   <si>
-    <t>Software testing, Building an ABM</t>
-  </si>
-  <si>
     <t>Project work: Implementing your own ABM</t>
   </si>
   <si>
     <t>Break for the evening (Homework: 1 slide description of model progress)</t>
   </si>
   <si>
-    <t>Discussion: Model building</t>
-  </si>
-  <si>
     <t>Homework presentations</t>
   </si>
   <si>
     <t>Chpts. 8,10,13</t>
   </si>
   <si>
-    <t>Design concepts: Agent sets, emergence, sensing, interactions</t>
-  </si>
-  <si>
     <t>Wild Dog Model</t>
   </si>
   <si>
-    <t>Adaptive behavior, Scheduling, collectives</t>
-  </si>
-  <si>
     <t>Chpts. 11, 14, 16</t>
   </si>
   <si>
@@ -166,19 +139,49 @@
     <t>Supplemental, Ch. 15</t>
   </si>
   <si>
-    <t>Break for evening (Homework: prepare presenation)</t>
-  </si>
-  <si>
     <t>Project work &amp; presentation prep</t>
   </si>
   <si>
     <t>Project Presentations &amp; Discussion</t>
   </si>
   <si>
-    <t>Uncertainty (Dr. Adam Duarte)</t>
-  </si>
-  <si>
-    <t>Becoming a modeler (Ms. Carra Carrillo)</t>
+    <t>Design presentations (1 slide)</t>
+  </si>
+  <si>
+    <t>Ch. 16</t>
+  </si>
+  <si>
+    <t>Break for evening (Homework: prepare presentation)</t>
+  </si>
+  <si>
+    <t>Lecture 01: What are models? Why do we use them? Intro to Netlogo</t>
+  </si>
+  <si>
+    <t>Lecture 02: Conceptual Modeling</t>
+  </si>
+  <si>
+    <t>Lecture 03: Software testing, Building an ABM</t>
+  </si>
+  <si>
+    <t>Exercise: building an ABM</t>
+  </si>
+  <si>
+    <t>Lecture 04: Design concepts: Agent sets, emergence, sensing, interactions</t>
+  </si>
+  <si>
+    <t>Lecture 05: Becoming a modeler (Ms. Carra Carrillo)</t>
+  </si>
+  <si>
+    <t>Lecture 06: Adaptive behavior, scheduling, collectives</t>
+  </si>
+  <si>
+    <t>Lecture 07: Model Evaluation &amp; pattern oriented modeling</t>
+  </si>
+  <si>
+    <t>Lecture 08:Uncertainty (Dr. Adam Duarte)</t>
+  </si>
+  <si>
+    <t>Lecture 09: Communicating and documenting models</t>
   </si>
 </sst>
 </file>
@@ -563,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D17388-0892-46A4-A8A8-F008C261F5AF}">
   <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +575,7 @@
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="77" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -597,7 +600,7 @@
         <v>800</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -606,10 +609,10 @@
         <v>900</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -618,7 +621,7 @@
         <v>1000</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -627,7 +630,7 @@
         <v>1130</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>5</v>
@@ -648,7 +651,7 @@
         <v>1330</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -657,7 +660,7 @@
         <v>1500</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4"/>
     </row>
@@ -667,10 +670,10 @@
         <v>1630</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -679,7 +682,7 @@
         <v>1700</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -696,7 +699,7 @@
         <v>800</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -705,19 +708,19 @@
         <v>915</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="3">
-        <v>1130</v>
+        <v>1000</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -729,16 +732,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="3">
         <v>1300</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>35</v>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -747,16 +750,16 @@
         <v>1400</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="3">
-        <v>1600</v>
+        <v>1430</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -765,7 +768,7 @@
         <v>1700</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -781,19 +784,19 @@
         <v>800</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="3">
         <v>900</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>37</v>
+      <c r="D22" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -802,7 +805,10 @@
         <v>1000</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -814,16 +820,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="3">
         <v>1300</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>25</v>
+      <c r="D25" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -841,7 +847,7 @@
         <v>1600</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -850,7 +856,7 @@
         <v>1700</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -866,19 +872,19 @@
         <v>800</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="C31" s="3">
         <v>900</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>46</v>
+      <c r="D31" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -900,16 +906,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="3">
         <v>1300</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -918,7 +924,7 @@
         <v>1330</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -927,7 +933,7 @@
         <v>1600</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -936,7 +942,7 @@
         <v>1700</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -946,13 +952,13 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C39" s="3">
         <v>800</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -970,7 +976,7 @@
         <v>1300</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -979,7 +985,7 @@
         <v>1600</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Todd's updated lectures, literature, models, and error cheat sheet
</commit_message>
<xml_diff>
--- a/ABM_Syllabus.xlsx
+++ b/ABM_Syllabus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Desktop\OSU_Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00469F7A-9500-422A-9F18-1C870D176161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AFB498-F311-46E8-93A8-AEE8AFF8CC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="135" windowWidth="28950" windowHeight="15465" xr2:uid="{E5130AA3-D4D3-4EA2-831A-5461D6EB2535}"/>
+    <workbookView xWindow="17295" yWindow="75" windowWidth="25065" windowHeight="14925" xr2:uid="{E5130AA3-D4D3-4EA2-831A-5461D6EB2535}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,29 +166,29 @@
     <t>Exercise: building an ABM</t>
   </si>
   <si>
-    <t>Lecture 04: Design concepts: Agent sets, emergence, sensing, interactions</t>
-  </si>
-  <si>
     <t>Lecture 05: Becoming a modeler (Ms. Carra Carrillo)</t>
   </si>
   <si>
     <t>Lecture 06: Adaptive behavior, scheduling, collectives</t>
   </si>
   <si>
-    <t>Lecture 07: Model Evaluation &amp; pattern oriented modeling</t>
-  </si>
-  <si>
     <t>Lecture 08:Uncertainty (Dr. Adam Duarte)</t>
   </si>
   <si>
     <t>Lecture 09: Communicating and documenting models</t>
+  </si>
+  <si>
+    <t>Lecture 07: Model evaluation &amp; pattern oriented modeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture 04: Design concepts &amp; programming tips </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,14 +200,23 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,14 +239,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -247,6 +254,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -567,15 +575,17 @@
   <dimension ref="B1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -592,8 +602,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3">
@@ -603,8 +613,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="6"/>
+    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
       <c r="C3" s="3">
         <v>900</v>
       </c>
@@ -615,8 +625,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
+    <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
       <c r="C4" s="3">
         <v>1000</v>
       </c>
@@ -624,8 +634,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
       <c r="C5" s="3">
         <v>1130</v>
       </c>
@@ -636,8 +646,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
       <c r="C6" s="3">
         <v>1230</v>
       </c>
@@ -645,8 +655,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
+    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
       <c r="C7" s="3">
         <v>1330</v>
       </c>
@@ -654,8 +664,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
       <c r="C8" s="3">
         <v>1500</v>
       </c>
@@ -664,8 +674,8 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
+    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
       <c r="C9" s="3">
         <v>1630</v>
       </c>
@@ -676,8 +686,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
       <c r="C10" s="3">
         <v>1700</v>
       </c>
@@ -685,14 +695,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3">
@@ -702,8 +712,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
       <c r="C13" s="3">
         <v>915</v>
       </c>
@@ -714,8 +724,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
+    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
       <c r="C14" s="3">
         <v>1000</v>
       </c>
@@ -723,8 +733,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
+    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
       <c r="C15" s="3">
         <v>1200</v>
       </c>
@@ -733,28 +743,28 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="3">
         <v>1300</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>43</v>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
+    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
       <c r="C17" s="3">
         <v>1400</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
+      <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
       <c r="C18" s="3">
         <v>1430</v>
       </c>
@@ -762,8 +772,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
       <c r="C19" s="3">
         <v>1700</v>
       </c>
@@ -771,13 +781,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
+    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
       <c r="C20" s="3"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="3">
@@ -788,31 +798,31 @@
       </c>
     </row>
     <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="3">
         <v>900</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
+    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
       <c r="C23" s="3">
         <v>1000</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
+    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
       <c r="C24" s="3">
         <v>1200</v>
       </c>
@@ -821,19 +831,19 @@
       </c>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="3">
         <v>1300</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
+    <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
       <c r="C26" s="3">
         <v>1400</v>
       </c>
@@ -841,8 +851,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
+    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
       <c r="C27" s="3">
         <v>1600</v>
       </c>
@@ -850,8 +860,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
+    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
       <c r="C28" s="3">
         <v>1700</v>
       </c>
@@ -859,13 +869,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
+    <row r="29" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="3">
@@ -876,19 +886,19 @@
       </c>
     </row>
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="3">
         <v>900</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
+    <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
       <c r="C32" s="3">
         <v>1000</v>
       </c>
@@ -897,8 +907,8 @@
       </c>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
+    <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
       <c r="C33" s="3">
         <v>1200</v>
       </c>
@@ -907,19 +917,19 @@
       </c>
     </row>
     <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="3">
         <v>1300</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>48</v>
+      <c r="D34" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="6"/>
+    <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
       <c r="C35" s="3">
         <v>1330</v>
       </c>
@@ -927,8 +937,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="6"/>
+    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
       <c r="C36" s="3">
         <v>1600</v>
       </c>
@@ -936,8 +946,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
+    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
       <c r="C37" s="3">
         <v>1700</v>
       </c>
@@ -945,13 +955,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
+    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
       <c r="C38" s="3"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
+    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="3">
@@ -961,8 +971,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="6"/>
+    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="7"/>
       <c r="C40" s="3">
         <v>1200</v>
       </c>
@@ -970,8 +980,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="6"/>
+    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="7"/>
       <c r="C41" s="3">
         <v>1300</v>
       </c>
@@ -979,8 +989,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="6"/>
+    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="7"/>
       <c r="C42" s="3">
         <v>1600</v>
       </c>
@@ -993,8 +1003,8 @@
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="B12:B19"/>
     <mergeCell ref="B21:B28"/>
-    <mergeCell ref="B30:B36"/>
     <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B30:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>